<commit_message>
Update distance 5260 AR
</commit_message>
<xml_diff>
--- a/Distance til 3 nodes 20 forsendelser PivotLonger.xlsx
+++ b/Distance til 3 nodes 20 forsendelser PivotLonger.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\402137\Desktop\Jonas Studie\SpecialePOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Github/Network-Analysis-Speciale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7E36EA-CDBA-4A61-830E-85A909AEA383}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0409555E-EB39-D64B-A8E9-382642721980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25275" yWindow="2670" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{592362EC-B083-4A7D-AC7B-7EC7DE312A7A}"/>
+    <workbookView xWindow="-76800" yWindow="-2220" windowWidth="38400" windowHeight="21600" xr2:uid="{592362EC-B083-4A7D-AC7B-7EC7DE312A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Distancer" sheetId="1" r:id="rId1"/>
@@ -843,24 +843,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA66F95-75A3-489E-94F6-6454CF91952E}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>140</v>
       </c>
@@ -889,7 +889,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
@@ -918,7 +918,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -947,7 +947,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>15</v>
       </c>
@@ -976,7 +976,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>17</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>13</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>19</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>7.6</v>
       </c>
       <c r="G18" s="2">
-        <v>69.7</v>
+        <v>141</v>
       </c>
       <c r="H18" s="2">
         <v>154</v>
@@ -1382,7 +1382,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>17</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>19</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>10</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>12</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>14</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>11</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>8</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>18</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>7</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>16</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2059,13 +2059,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C00E91B-7C4C-4C3A-9D0E-D69B706E90F2}">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>145</v>
       </c>

</xml_diff>